<commit_message>
update test 03: Order Management
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,9 +408,23 @@
         <v>ba4149f313130fa829e84292f3fdbd74680b4f363e5f4ec6ea1cd73cde529b6d</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>16.03.2023</v>
+      </c>
+      <c r="C3" t="str">
+        <v>https://gitlab.intra.infineon.com/digital-reference/order_management/-/commit/47cbb7faff327805f4f0ae6f71ccbeec1e086e96</v>
+      </c>
+      <c r="D3" t="str">
+        <v>b67d5d8d24cae366f52cd197bc9be1e731229e148dc25959342bb7020c3a6bd0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
system for layered ontology
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,9 +408,23 @@
         <v>ba4149f313130fa829e84292f3fdbd74680b4f363e5f4ec6ea1cd73cde529b6d</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>16.03.2023</v>
+      </c>
+      <c r="C3" t="str">
+        <v>https://gitlab.intra.infineon.com/digital-reference/order_management/-/commit/47cbb7faff327805f4f0ae6f71ccbeec1e086e96</v>
+      </c>
+      <c r="D3" t="str">
+        <v>b67d5d8d24cae366f52cd197bc9be1e731229e148dc25959342bb7020c3a6bd0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update and change timestamp in closed proposal
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,9 +422,23 @@
         <v>b67d5d8d24cae366f52cd197bc9be1e731229e148dc25959342bb7020c3a6bd0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>23.03.2023 10:09 (CET)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/4f24e65057a7257c057b4ab9241d4c02154082ae</v>
+      </c>
+      <c r="D4" t="str">
+        <v>54d4d2f24ac8d7a88ec095deed5ffb07daab728d3a812d4d0503aacf7cd69912</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test 07, 08
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,9 +436,23 @@
         <v>54d4d2f24ac8d7a88ec095deed5ffb07daab728d3a812d4d0503aacf7cd69912</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>24.03.2023 15:41 (CET)</v>
+      </c>
+      <c r="C5" t="str">
+        <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/fb965955f5d3cc29931426bf15edfcd279305895</v>
+      </c>
+      <c r="D5" t="str">
+        <v>b95ad415b600b67a1ceb8669c0838ed63b287ee61121c14e73fa33c6d73200af</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sync ledger and blockchain
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +405,7 @@
         <v>https://gitlab.intra.infineon.com/digital-reference/order_management/-/commit/802222735fe9a7fa2b0feb3ad198dbbb30342ac9</v>
       </c>
       <c r="D2" t="str">
-        <v>38e095848ec25b80ff89be18825606c120ad93542e03c2755eb84ee90edfe5b5</v>
+        <v>ba4149f313130fa829e84292f3fdbd74680b4f363e5f4ec6ea1cd73cde529b6d</v>
       </c>
     </row>
     <row r="3">
@@ -419,12 +419,54 @@
         <v>https://gitlab.intra.infineon.com/digital-reference/order_management/-/commit/47cbb7faff327805f4f0ae6f71ccbeec1e086e96</v>
       </c>
       <c r="D3" t="str">
-        <v>245d2c837d0ca60011818cdb9aded89abfb4d4f5eb94148440124e43d291921d</v>
+        <v>b67d5d8d24cae366f52cd197bc9be1e731229e148dc25959342bb7020c3a6bd0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>23.03.2023 10:09 (CET)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/4f24e65057a7257c057b4ab9241d4c02154082ae</v>
+      </c>
+      <c r="D4" t="str">
+        <v>54d4d2f24ac8d7a88ec095deed5ffb07daab728d3a812d4d0503aacf7cd69912</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>24.03.2023 15:41 (CET)</v>
+      </c>
+      <c r="C5" t="str">
+        <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/fb965955f5d3cc29931426bf15edfcd279305895</v>
+      </c>
+      <c r="D5" t="str">
+        <v>b95ad415b600b67a1ceb8669c0838ed63b287ee61121c14e73fa33c6d73200af</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>31.03.2023 12:34 (CET)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/e62a015a27d3885eca648a019cb9616469209ed4</v>
+      </c>
+      <c r="D6" t="str">
+        <v>13fe359073f7923d47d052271661c1c01948ff2ded7719cb70a3603a88e43676</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test 11 layered
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -405,7 +405,7 @@
         <v>https://gitlab.intra.infineon.com/digital-reference/order_management/-/commit/802222735fe9a7fa2b0feb3ad198dbbb30342ac9</v>
       </c>
       <c r="D2" t="str">
-        <v>ba4149f313130fa829e84292f3fdbd74680b4f363e5f4ec6ea1cd73cde529b6d</v>
+        <v>38e095848ec25b80ff89be18825606c120ad93542e03c2755eb84ee90edfe5b5</v>
       </c>
     </row>
     <row r="3">
@@ -419,7 +419,7 @@
         <v>https://gitlab.intra.infineon.com/digital-reference/order_management/-/commit/47cbb7faff327805f4f0ae6f71ccbeec1e086e96</v>
       </c>
       <c r="D3" t="str">
-        <v>b67d5d8d24cae366f52cd197bc9be1e731229e148dc25959342bb7020c3a6bd0</v>
+        <v>245d2c837d0ca60011818cdb9aded89abfb4d4f5eb94148440124e43d291921d</v>
       </c>
     </row>
     <row r="4">
@@ -433,7 +433,7 @@
         <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/4f24e65057a7257c057b4ab9241d4c02154082ae</v>
       </c>
       <c r="D4" t="str">
-        <v>54d4d2f24ac8d7a88ec095deed5ffb07daab728d3a812d4d0503aacf7cd69912</v>
+        <v>1a69917e78ae842865dfb5571a62d65494a59aac74a48f31f3bb799425cdf535</v>
       </c>
     </row>
     <row r="5">
@@ -447,7 +447,7 @@
         <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/fb965955f5d3cc29931426bf15edfcd279305895</v>
       </c>
       <c r="D5" t="str">
-        <v>b95ad415b600b67a1ceb8669c0838ed63b287ee61121c14e73fa33c6d73200af</v>
+        <v>915b10f800bf6b1db00913183b44f454e0b4daa910915de907369297ff61dcda</v>
       </c>
     </row>
     <row r="6">
@@ -461,7 +461,7 @@
         <v>https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/e62a015a27d3885eca648a019cb9616469209ed4</v>
       </c>
       <c r="D6" t="str">
-        <v>13fe359073f7923d47d052271661c1c01948ff2ded7719cb70a3603a88e43676</v>
+        <v>6b11204cfb0ef5ded49c9bad3ecf995a34c45a0c7a33ea388da12f409b750f73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test 11, 12
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,9 +464,23 @@
         <v>13fe359073f7923d47d052271661c1c01948ff2ded7719cb70a3603a88e43676</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>17.04.2023 12:44 (CET)</v>
+      </c>
+      <c r="C7" t="str">
+        <v>{"ProposedVersion":"https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/50873a28b7e97ba8d65492c7a7938f0fc336ac02","UpdatedVersion":"https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/90c783a6e4ff122dbc160ccf0a2745e78a024c73","Domain":"Supply Chain","LobeOwner":"member1","Result":"accept by lobe owner"}</v>
+      </c>
+      <c r="D7" t="str">
+        <v>ee13b88d68beaeeaa2e325de2be50a5cebb5d9b211a1498d3ae932d37a28e310</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test 11, 12 using layered system
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_OrderManagement.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,9 +464,23 @@
         <v>6b11204cfb0ef5ded49c9bad3ecf995a34c45a0c7a33ea388da12f409b750f73</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>17.04.2023 12:44 (CET)</v>
+      </c>
+      <c r="C7" t="str">
+        <v>{"ProposedVersion":"https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/50873a28b7e97ba8d65492c7a7938f0fc336ac02","UpdatedVersion":"https://gitlab.intra.infineon.com/semantic-web-projects/digital-reference/order_management/-/commit/90c783a6e4ff122dbc160ccf0a2745e78a024c73","Domain":"Supply Chain","LobeOwner":"member1","Result":"accept by lobe owner"}</v>
+      </c>
+      <c r="D7" t="str">
+        <v>3eabfa48eb39069846a1b161e3d2f19b23a539121e9fdd3692294e375171601c</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>